<commit_message>
Files Sent to sierra for production Build
</commit_message>
<xml_diff>
--- a/Financials.xlsx
+++ b/Financials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="26835" windowHeight="12330"/>
+    <workbookView xWindow="705" yWindow="4050" windowWidth="26835" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>QTY</t>
   </si>
@@ -35,13 +35,43 @@
   </si>
   <si>
     <t>Total Profit</t>
+  </si>
+  <si>
+    <t>PCB Cost</t>
+  </si>
+  <si>
+    <t>Assy Cost</t>
+  </si>
+  <si>
+    <t>BOM Cost</t>
+  </si>
+  <si>
+    <t>P470HCT-ND</t>
+  </si>
+  <si>
+    <t>P330HCT-ND</t>
+  </si>
+  <si>
+    <t>APL3015SGC-F01</t>
+  </si>
+  <si>
+    <t>10018783=10203TLF</t>
+  </si>
+  <si>
+    <t>Sierra Circuits</t>
+  </si>
+  <si>
+    <t>Total investment</t>
+  </si>
+  <si>
+    <t>Break Even units</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,16 +86,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,14 +121,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,19 +441,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,11 +473,11 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>250</v>
       </c>
@@ -433,12 +499,13 @@
         <f>(D2/C2)-1</f>
         <v>0.39527779246491224</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1"/>
+      <c r="H2">
         <f>(D2-C2)*A2</f>
         <v>1345.6599999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>500</v>
       </c>
@@ -460,12 +527,13 @@
         <f t="shared" ref="F3:F4" si="2">(D3/C3)-1</f>
         <v>0.35539555863983341</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G4" si="3">(D3-C3)*A3</f>
+      <c r="G3" s="1"/>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="3">(D3-C3)*A3</f>
         <v>2294.3199999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -487,18 +555,235 @@
         <f t="shared" si="2"/>
         <v>0.28236100034085987</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1"/>
+      <c r="H4">
         <f t="shared" si="3"/>
         <v>3412.9199999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <f>D4/C4</f>
         <v>1.2823610003408599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>250</v>
+      </c>
+      <c r="B12">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="C12">
+        <v>5.71</v>
+      </c>
+      <c r="D12">
+        <f>E22</f>
+        <v>1.6267199999999999</v>
+      </c>
+      <c r="E12">
+        <f>SUM(B12:D12)*1.08</f>
+        <v>12.632457600000002</v>
+      </c>
+      <c r="F12">
+        <v>19</v>
+      </c>
+      <c r="G12">
+        <f>15*(0.04)</f>
+        <v>0.6</v>
+      </c>
+      <c r="H12">
+        <f>(F12/E12)-1</f>
+        <v>0.50406204411087807</v>
+      </c>
+      <c r="I12">
+        <f>A12*(F12-E12)</f>
+        <v>1591.8855999999994</v>
+      </c>
+      <c r="K12">
+        <f>E12*A12</f>
+        <v>3158.1144000000004</v>
+      </c>
+      <c r="M12">
+        <f>ROUND((E12/F12)*A12,0)</f>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>500</v>
+      </c>
+      <c r="B13">
+        <v>4.01</v>
+      </c>
+      <c r="C13">
+        <v>4.62</v>
+      </c>
+      <c r="D13">
+        <f>F22</f>
+        <v>1.52928</v>
+      </c>
+      <c r="E13">
+        <f>SUM(B13:D13)*1.08</f>
+        <v>10.9720224</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <f>(F13/E13)-1</f>
+        <v>0.36711350498154283</v>
+      </c>
+      <c r="I13">
+        <f>A13*(F13-E13)</f>
+        <v>2013.9887999999999</v>
+      </c>
+      <c r="K13">
+        <f>E13*A13</f>
+        <v>5486.0111999999999</v>
+      </c>
+      <c r="M13">
+        <f>ROUND((E13/F13)*A13,0)</f>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="D17">
+        <v>5.7600000000000004E-3</v>
+      </c>
+      <c r="E17">
+        <f>A17*C17</f>
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="F17">
+        <f>D17*A17</f>
+        <v>5.7600000000000004E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="D18">
+        <v>5.7600000000000004E-3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:E20" si="4">A18*C18</f>
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ref="F18:F20" si="5">D18*A18</f>
+        <v>5.7600000000000004E-3</v>
+      </c>
+      <c r="H18">
+        <f>50*13</f>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>0.09</v>
+      </c>
+      <c r="D19">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
+        <v>0.18</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>0.16200000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>0.71555999999999997</v>
+      </c>
+      <c r="D20">
+        <v>0.67788000000000004</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>1.4311199999999999</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>1.3557600000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="E22">
+        <f>SUM(E17:E20)</f>
+        <v>1.6267199999999999</v>
+      </c>
+      <c r="F22">
+        <f>SUM(F17:F20)</f>
+        <v>1.52928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>